<commit_message>
Make IXLCell.GetFormattedString() more compliant with Excel. Custom formats are only for number, not other types, like text, bools or error.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/CellValues.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/CellValues.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <x:si>
     <x:t>Initial Value</x:t>
   </x:si>
@@ -42,9 +42,6 @@
   </x:si>
   <x:si>
     <x:t>TRUE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>True</x:t>
   </x:si>
   <x:si>
     <x:t>1234.567</x:t>
@@ -539,7 +536,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="G4" s="4" t="s">
-        <x:v>9</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
@@ -556,30 +553,30 @@
         <x:v>1234.567</x:v>
       </x:c>
       <x:c r="F5" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G5" s="4" t="s">
         <x:v>10</x:v>
-      </x:c>
-      <x:c r="G5" s="4" t="s">
-        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="B6" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
@@ -596,10 +593,10 @@
         <x:v>1.10538194444444</x:v>
       </x:c>
       <x:c r="F7" s="4" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="G7" s="4" t="s">
-        <x:v>13</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -624,7 +621,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="4" t="s">
-        <x:v>14</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Implement loading/saving of error values.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/CellValues.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/CellValues.xlsx
@@ -8,6 +8,7 @@
   <x:sheets>
     <x:sheet name="Cell Values" sheetId="2" r:id="rId2"/>
     <x:sheet name="Test Whitespace" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Errors" sheetId="4" r:id="rId4"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <x:si>
     <x:t>Initial Value</x:t>
   </x:si>
@@ -56,7 +57,16 @@
     <x:t>26:31:45</x:t>
   </x:si>
   <x:si>
+    <x:t>#DIV/0!</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">    </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Error value</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Formula error</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -464,7 +474,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G7"/>
+  <x:dimension ref="A1:G8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -597,6 +607,26 @@
       </x:c>
       <x:c r="G7" s="4" t="s">
         <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:7">
+      <x:c r="B8" s="0" t="e">
+        <x:v>#DIV/0!</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="e">
+        <x:v>#DIV/0!</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="e">
+        <x:v>#DIV/0!</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="e">
+        <x:v>#DIV/0!</x:v>
+      </x:c>
+      <x:c r="F8" s="4" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="G8" s="4" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -621,7 +651,98 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="4" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C9"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="2" spans="1:3">
+      <x:c r="B2" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="B3" s="0" t="e">
+        <x:v>#REF!</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="e">
+        <x:f>#REF!+1</x:f>
+        <x:v>#REF!</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="B4" s="0" t="e">
+        <x:v>#VALUE!</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="e">
+        <x:f>"TRUE"*1</x:f>
+        <x:v>#VALUE!</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="B5" s="0" t="e">
+        <x:v>#DIV/0!</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="e">
+        <x:f>1/0</x:f>
+        <x:v>#DIV/0!</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="B6" s="0" t="e">
+        <x:v>#NAME?</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="e">
+        <x:f>NONEXISTENT.FUNCTION()</x:f>
+        <x:v>#NAME?</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:3">
+      <x:c r="B7" s="0" t="e">
+        <x:v>#N/A</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="e">
+        <x:f>NA()</x:f>
+        <x:v>#N/A</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
+      <x:c r="B8" s="0" t="e">
+        <x:v>#NULL!</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="e">
+        <x:f>#NULL!+1</x:f>
+        <x:v>#NULL!</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3">
+      <x:c r="B9" s="0" t="e">
+        <x:v>#NUM!</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="e">
+        <x:f>#NUM!+1</x:f>
+        <x:v>#NUM!</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>